<commit_message>
Updated checklist and create_tables.sql
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Checklist</t>
   </si>
@@ -59,12 +59,6 @@
     <t>9. Spreadsheet Display</t>
   </si>
   <si>
-    <t>10. Account creation page</t>
-  </si>
-  <si>
-    <t>11. Change Account info page</t>
-  </si>
-  <si>
     <t>Accomplished?</t>
   </si>
   <si>
@@ -74,7 +68,16 @@
     <t>X</t>
   </si>
   <si>
-    <t>12. Mentor--Student linking Page</t>
+    <t>10. Create Company page</t>
+  </si>
+  <si>
+    <t>11. Account creation page</t>
+  </si>
+  <si>
+    <t>12. Change Account info page</t>
+  </si>
+  <si>
+    <t>13. Mentor--Student linking Page</t>
   </si>
 </sst>
 </file>
@@ -395,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,74 +421,103 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added student-mentor link pages and updated checklist
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Checklist</t>
   </si>
@@ -401,7 +401,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,13 +508,17 @@
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>

</xml_diff>

<commit_message>
Edited homepage to include links to other pages
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Checklist</t>
   </si>
@@ -401,7 +401,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +440,9 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -468,7 +470,9 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>

<commit_message>
Fixed student - mentor linking page
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -86,10 +86,10 @@
     <t>15. Database Wipe</t>
   </si>
   <si>
-    <t>16. Mentor - Student Display</t>
-  </si>
-  <si>
     <t>17. Statement of work</t>
+  </si>
+  <si>
+    <t>16. Form status list</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,12 +555,12 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>